<commit_message>
update for all PSYC modules
</commit_message>
<xml_diff>
--- a/URL_Rules.xlsx
+++ b/URL_Rules.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Human" sheetId="1" r:id="rId1"/>
     <sheet name="Machine" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" iterateDelta="252" concurrentCalc="0"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>HPSC</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>https://www.ucl.ac.uk/geography/open-pages/mdc-module-view.php?module=%s</t>
+  </si>
+  <si>
+    <t>https://www.ucl.ac.uk/lifesciences-faculty-php/courses/viewcourse.php?coursecode=%s</t>
+  </si>
+  <si>
+    <t>PSYC.*</t>
+  </si>
+  <si>
+    <t>PSYC</t>
   </si>
 </sst>
 </file>
@@ -561,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,12 +835,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C6" r:id="rId2"/>
     <hyperlink ref="C18" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
+    <hyperlink ref="C20" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add number of students on modules from BoE reports
</commit_message>
<xml_diff>
--- a/URL_Rules.xlsx
+++ b/URL_Rules.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
   <si>
     <t>HPSC</t>
   </si>
@@ -114,18 +114,9 @@
     <t>MATH (Y1)</t>
   </si>
   <si>
-    <t>MATH(1).*</t>
-  </si>
-  <si>
     <t>http://www.ucl.ac.uk/maths/courses/undergraduates/modules/year1/year1_syllabuses/%s</t>
   </si>
   <si>
-    <t>thing[5]</t>
-  </si>
-  <si>
-    <t>PHAS</t>
-  </si>
-  <si>
     <t>ANTH.*</t>
   </si>
   <si>
@@ -177,9 +168,6 @@
     <t>https://www.ucl.ac.uk/maths/courses/undergraduates/modules/year3/year3_syllabuses/%s</t>
   </si>
   <si>
-    <t>http://www.ucl.ac.uk/physics-astronomy/intranet/student-intranet/undergraduate/y%s_Descriptions</t>
-  </si>
-  <si>
     <t>http://www.ucl.ac.uk/anthropology/courses/ug/%s</t>
   </si>
   <si>
@@ -207,9 +195,6 @@
     <t>MATH3.*</t>
   </si>
   <si>
-    <t>PHAS[1-4].*</t>
-  </si>
-  <si>
     <t>https://www.ucl.ac.uk/geography/open-pages/mdc-module-view.php?module=%s</t>
   </si>
   <si>
@@ -256,6 +241,120 @@
   </si>
   <si>
     <t>http://www.ucl.ac.uk/earth-sciences/study/undergraduate/modules/%s</t>
+  </si>
+  <si>
+    <t>MATH1.*</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/physics-astronomy/intranet/current-students/undergraduate/2nd-year-module-descriptions-17-18</t>
+  </si>
+  <si>
+    <t>PHAS1.*</t>
+  </si>
+  <si>
+    <t>PHAS2.*</t>
+  </si>
+  <si>
+    <t>PHAS3.*</t>
+  </si>
+  <si>
+    <t>PHAS4.*</t>
+  </si>
+  <si>
+    <t>PHAS (Y1)</t>
+  </si>
+  <si>
+    <t>PHAS (Y2)</t>
+  </si>
+  <si>
+    <t>PHAS (Y3)</t>
+  </si>
+  <si>
+    <t>PHAS (Y4)</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/physics-astronomy/intranet/current-students/undergraduate/1st-year-module-descriptions-17-18</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/physics-astronomy/intranet/current-students/undergraduate/3rd-year-module-descriptions-17-18</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/physics-astronomy/intranet/current-students/undergraduate/4th-year-module-descriptions-17-18</t>
+  </si>
+  <si>
+    <t>BASC1001</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/atk</t>
+  </si>
+  <si>
+    <t>BASC1002</t>
+  </si>
+  <si>
+    <t>BASC1003</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/qm</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/irm</t>
+  </si>
+  <si>
+    <t>BASC2001</t>
+  </si>
+  <si>
+    <t>BASC2002</t>
+  </si>
+  <si>
+    <t>BASC2003</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/ol</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/qm2</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/qt</t>
+  </si>
+  <si>
+    <t>BASC (IE)</t>
+  </si>
+  <si>
+    <t>BASC2.*</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/ie/%s</t>
+  </si>
+  <si>
+    <t>BASC3001</t>
+  </si>
+  <si>
+    <t>BASC3002</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/core/dissertation</t>
+  </si>
+  <si>
+    <t>ANTH1017</t>
+  </si>
+  <si>
+    <t>ANTH(1017|7034)</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/basc/current/pathways/cultures/%s</t>
+  </si>
+  <si>
+    <t>BASC2004</t>
+  </si>
+  <si>
+    <t>http://www.ucl.ac.uk/philosophy/current-students/ba-programmes/ba-modules</t>
+  </si>
+  <si>
+    <t>PHIL</t>
+  </si>
+  <si>
+    <t>PHIL.*</t>
   </si>
 </sst>
 </file>
@@ -310,7 +409,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -318,16 +417,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -606,32 +709,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="108" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -650,13 +753,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -681,10 +784,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -709,10 +812,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -720,102 +823,96 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
+        <v>73</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
+        <v>76</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
@@ -823,258 +920,447 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" t="s">
-        <v>4</v>
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f>_xlfn.CONCAT(A21,".*")</f>
-        <v>ANAT.*</v>
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f t="shared" ref="B22:B32" si="0">_xlfn.CONCAT(A22,".*")</f>
-        <v>BIOC.*</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>61</v>
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="1" t="str">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f>_xlfn.CONCAT(A24,".*")</f>
+        <v>ANAT.*</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f t="shared" ref="B25:B35" si="0">_xlfn.CONCAT(A25,".*")</f>
+        <v>BIOC.*</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>BIOL.*</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="1" t="str">
+      <c r="C26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NEUR.*</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="1" t="str">
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PHAR.*</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="1" t="str">
+      <c r="C28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PHOL.*</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="1" t="str">
+      <c r="C29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>BIOS.*</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="1" t="str">
+      <c r="C30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>CELL.*</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="1" t="str">
+      <c r="C31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NEUR.*</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="1" t="str">
+      <c r="C32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PALS.*</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="1" t="str">
+      <c r="C33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PHAY.*</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="1" t="str">
+      <c r="C34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>GEOL.*</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C6" r:id="rId2"/>
-    <hyperlink ref="C18" r:id="rId3"/>
+    <hyperlink ref="C21" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C20" r:id="rId5"/>
-    <hyperlink ref="C21:C26" r:id="rId6" display="https://www.ucl.ac.uk/lifesciences-faculty-php/courses/viewcourse.php?coursecode=%s"/>
-    <hyperlink ref="C27:C31" r:id="rId7" display="https://www.ucl.ac.uk/lifesciences-faculty-php/courses/viewcourse.php?coursecode=%s"/>
-    <hyperlink ref="C32" r:id="rId8"/>
+    <hyperlink ref="C23" r:id="rId5"/>
+    <hyperlink ref="C24:C29" r:id="rId6" display="https://www.ucl.ac.uk/lifesciences-faculty-php/courses/viewcourse.php?coursecode=%s"/>
+    <hyperlink ref="C30:C34" r:id="rId7" display="https://www.ucl.ac.uk/lifesciences-faculty-php/courses/viewcourse.php?coursecode=%s"/>
+    <hyperlink ref="C35" r:id="rId8"/>
+    <hyperlink ref="C8" r:id="rId9"/>
+    <hyperlink ref="C10" r:id="rId10"/>
+    <hyperlink ref="C11" r:id="rId11"/>
+    <hyperlink ref="C37" r:id="rId12"/>
+    <hyperlink ref="C40" r:id="rId13"/>
+    <hyperlink ref="C41" r:id="rId14"/>
+    <hyperlink ref="C42" r:id="rId15"/>
+    <hyperlink ref="C39" r:id="rId16"/>
+    <hyperlink ref="C43" r:id="rId17"/>
+    <hyperlink ref="C44" r:id="rId18"/>
+    <hyperlink ref="C45" r:id="rId19"/>
+    <hyperlink ref="C46" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1099,27 +1385,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>

</xml_diff>